<commit_message>
Add support for additional column types (#10)
</commit_message>
<xml_diff>
--- a/test/files/office365-xl7.xlsx
+++ b/test/files/office365-xl7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcult\Documents\Martijn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4E84D2A-7A46-4970-8A3A-9815B162BECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02B023B-9D83-4608-BAF5-47478CFF8FBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BB3C9F8E-181F-4080-A913-21C40A5BF3CB}"/>
   </bookViews>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>the</t>
   </si>
@@ -63,6 +65,12 @@
   </si>
   <si>
     <t>Date w/ time</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Boolean</t>
   </si>
 </sst>
 </file>
@@ -106,10 +114,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
@@ -487,18 +496,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FE69C7-1523-45B3-87E0-BB2F98A2A479}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -508,8 +518,14 @@
       <c r="C1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0.25</v>
       </c>
@@ -519,6 +535,17 @@
       </c>
       <c r="C2" s="2">
         <v>43881.555555555555</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43901</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>